<commit_message>
add text sign function
</commit_message>
<xml_diff>
--- a/public/signature.xlsx
+++ b/public/signature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachy\Desktop\pdf-form-filling\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD1AE8B-F580-409D-BB4D-5FF8E5B3F6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EEB4DA7-DF8A-493E-8A80-B6D7F07EBD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="2370" windowWidth="21840" windowHeight="15090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18120" yWindow="6345" windowWidth="21840" windowHeight="15090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Signature1</t>
-  </si>
-  <si>
-    <t>file://signature.png</t>
   </si>
 </sst>
 </file>
@@ -77,7 +74,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -366,6 +363,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -373,14 +373,11 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+      <c r="A2" s="1">
+        <v>123123</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{0339CA01-71A8-4B5B-9B58-706D9C84DDCC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>